<commit_message>
Update Pertanggal 8 Januari 2026 18:30 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorkerType.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorkerType.xlsx
@@ -780,8 +780,8 @@
   </sheetPr>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>